<commit_message>
Add Isipheko contribution to Mhlengi
</commit_message>
<xml_diff>
--- a/data/statement.xlsx
+++ b/data/statement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9D91F5C6FBD4D568/Documents/stokvel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsepo\App3\ezase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="8_{B450040B-8985-4461-A01C-67391E1711C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A685E95-B07C-4ABC-A3F2-A3AA587E493F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B372268-771A-404C-9DB5-F179C8EB6905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D931818-D3BD-4426-8858-9BFAAB080988}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Thabo</t>
+  </si>
+  <si>
+    <t>Isipheko</t>
   </si>
 </sst>
 </file>
@@ -149,10 +152,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,7 +475,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1474,24 +1473,89 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C59" s="1">
+        <v>45864</v>
+      </c>
+      <c r="D59" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="2">
+        <v>300</v>
+      </c>
+      <c r="C60" s="1">
+        <v>45864</v>
+      </c>
+      <c r="D60" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E60" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C61" s="1">
+        <v>45847</v>
+      </c>
+      <c r="D61" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
+      <c r="A62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C62" s="1">
+        <v>45847</v>
+      </c>
+      <c r="D62" s="1">
+        <v>45930</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="2">
+        <v>300</v>
+      </c>
+      <c r="C63" s="1">
+        <v>45847</v>
+      </c>
+      <c r="D63" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C64" s="1"/>

</xml_diff>

<commit_message>
Updated statement.x1sx with new data
</commit_message>
<xml_diff>
--- a/data/statement.xlsx
+++ b/data/statement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsepo\App3\ezase\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08968840-348F-4391-9808-FE3B3A1C50D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33A0CBA-F20D-46F2-81DB-EE452ED656B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D931818-D3BD-4426-8858-9BFAAB080988}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Isipheko</t>
+  </si>
+  <si>
+    <t>Penalty</t>
   </si>
 </sst>
 </file>
@@ -471,11 +474,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379A97FC-4855-4BBD-BC60-065F4E41B287}">
-  <dimension ref="A1:E372"/>
+  <dimension ref="A1:E370"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1592,44 +1595,174 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="A66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C66" s="1">
+        <v>45868</v>
+      </c>
+      <c r="D66" s="1">
+        <v>45961</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C67" s="1">
+        <v>45868</v>
+      </c>
+      <c r="D67" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C68" s="1">
+        <v>45871</v>
+      </c>
+      <c r="D68" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="2">
+        <v>550</v>
+      </c>
+      <c r="C69" s="1">
+        <v>45874</v>
+      </c>
+      <c r="D69" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="2">
+        <v>300</v>
+      </c>
+      <c r="C70" s="1">
+        <v>45874</v>
+      </c>
+      <c r="D70" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E70" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C71" s="1">
+        <v>45874</v>
+      </c>
+      <c r="D71" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" s="2">
+        <v>300</v>
+      </c>
+      <c r="C72" s="1">
+        <v>45874</v>
+      </c>
+      <c r="D72" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E72" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" s="2">
+        <v>20</v>
+      </c>
+      <c r="C73" s="1">
+        <v>45874</v>
+      </c>
+      <c r="D73" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E73" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C74" s="1">
+        <v>45874</v>
+      </c>
+      <c r="D74" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="2">
+        <v>300</v>
+      </c>
+      <c r="C75" s="1">
+        <v>45874</v>
+      </c>
+      <c r="D75" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E75" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C76" s="1"/>
@@ -1742,10 +1875,12 @@
     <row r="103" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
     </row>
     <row r="104" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
     </row>
     <row r="105" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C105" s="1"/>
@@ -3077,16 +3212,6 @@
       <c r="D370" s="1"/>
       <c r="E370" s="1"/>
     </row>
-    <row r="371" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C371" s="1"/>
-      <c r="D371" s="1"/>
-      <c r="E371" s="1"/>
-    </row>
-    <row r="372" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C372" s="1"/>
-      <c r="D372" s="1"/>
-      <c r="E372" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated app.py and statement.xlsx
</commit_message>
<xml_diff>
--- a/data/statement.xlsx
+++ b/data/statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsepo\App3\ezase\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33A0CBA-F20D-46F2-81DB-EE452ED656B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012DB587-3F49-490E-99F6-718BCC54CB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D931818-D3BD-4426-8858-9BFAAB080988}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0D931818-D3BD-4426-8858-9BFAAB080988}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -474,11 +474,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379A97FC-4855-4BBD-BC60-065F4E41B287}">
-  <dimension ref="A1:E370"/>
+  <dimension ref="A1:E367"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1765,86 +1765,242 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="2">
+        <v>3050</v>
+      </c>
+      <c r="C76" s="1">
+        <v>45894</v>
+      </c>
+      <c r="D76" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C77" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D77" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C78" s="1">
+        <v>45897</v>
+      </c>
+      <c r="D78" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>45835</v>
+      </c>
+      <c r="D79" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-    </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-    </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-    </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="2">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>45843</v>
+      </c>
+      <c r="D80" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="2">
+        <v>550</v>
+      </c>
+      <c r="C81" s="1">
+        <v>45898</v>
+      </c>
+      <c r="D81" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C82" s="1">
+        <v>45905</v>
+      </c>
+      <c r="D82" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C83" s="1">
+        <v>45898</v>
+      </c>
+      <c r="D83" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84" s="2">
+        <v>300</v>
+      </c>
+      <c r="C84" s="1">
+        <v>45898</v>
+      </c>
+      <c r="D84" s="1">
+        <v>45900</v>
+      </c>
+      <c r="E84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" s="2">
+        <v>50</v>
+      </c>
+      <c r="C85" s="1">
+        <v>45898</v>
+      </c>
+      <c r="D85" s="1">
+        <v>45869</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>9</v>
+      </c>
+      <c r="B86" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C86" s="1">
+        <v>45889</v>
+      </c>
+      <c r="D86" s="1">
+        <v>45991</v>
+      </c>
+      <c r="E86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="2">
+        <v>1050</v>
+      </c>
+      <c r="C87" s="1">
+        <v>45902</v>
+      </c>
+      <c r="D87" s="1">
+        <v>46022</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
@@ -1863,14 +2019,17 @@
     <row r="100" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
     </row>
     <row r="101" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
     </row>
     <row r="102" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
     </row>
     <row r="103" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C103" s="1"/>
@@ -3197,21 +3356,6 @@
       <c r="D367" s="1"/>
       <c r="E367" s="1"/>
     </row>
-    <row r="368" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C368" s="1"/>
-      <c r="D368" s="1"/>
-      <c r="E368" s="1"/>
-    </row>
-    <row r="369" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C369" s="1"/>
-      <c r="D369" s="1"/>
-      <c r="E369" s="1"/>
-    </row>
-    <row r="370" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C370" s="1"/>
-      <c r="D370" s="1"/>
-      <c r="E370" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>